<commit_message>
Con tiempos de junta 6
</commit_message>
<xml_diff>
--- a/swbproys/gestor-bsc/doc/LAU/formatos lanzamiento.xlsx
+++ b/swbproys/gestor-bsc/doc/LAU/formatos lanzamiento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="15240" windowHeight="5985" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="330" windowWidth="15240" windowHeight="5985" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GOAL" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="231">
   <si>
     <t>Measures</t>
   </si>
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,9 +1977,7 @@
       <c r="C4" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="69">
-        <v>0.11319444444444444</v>
-      </c>
+      <c r="D4" s="69"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2202,7 +2200,9 @@
       <c r="B33" s="39">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C33" s="39"/>
+      <c r="C33" s="39">
+        <v>0.8125</v>
+      </c>
       <c r="D33" s="54" t="s">
         <v>199</v>
       </c>
@@ -2210,8 +2210,12 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="49"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
+      <c r="B34" s="39">
+        <v>0.8125</v>
+      </c>
+      <c r="C34" s="39">
+        <v>0.83194444444444438</v>
+      </c>
       <c r="D34" s="54" t="s">
         <v>200</v>
       </c>
@@ -2219,8 +2223,12 @@
     </row>
     <row r="35" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="49"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
+      <c r="B35" s="39">
+        <v>0.83194444444444438</v>
+      </c>
+      <c r="C35" s="39">
+        <v>0.8354166666666667</v>
+      </c>
       <c r="D35" s="54" t="s">
         <v>201</v>
       </c>
@@ -2228,7 +2236,9 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="49"/>
-      <c r="B36" s="39"/>
+      <c r="B36" s="39">
+        <v>0.8354166666666667</v>
+      </c>
       <c r="C36" s="39"/>
       <c r="D36" s="54" t="s">
         <v>77</v>
@@ -2268,13 +2278,9 @@
       </c>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="B43" s="38" t="s">
-        <v>195</v>
-      </c>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="77"/>
       <c r="D43" s="77"/>
     </row>
@@ -6289,13 +6295,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -6620,13 +6626,16 @@
         <v>41439</v>
       </c>
       <c r="F22" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>160</v>
       </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
       <c r="F23" t="s">
         <v>107</v>
       </c>
@@ -6635,6 +6644,9 @@
       <c r="A24" t="s">
         <v>161</v>
       </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
       <c r="F24" t="s">
         <v>148</v>
       </c>
@@ -6643,6 +6655,9 @@
       <c r="A25" t="s">
         <v>162</v>
       </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
       <c r="F25" t="s">
         <v>148</v>
       </c>
@@ -6651,8 +6666,11 @@
       <c r="A26" t="s">
         <v>167</v>
       </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
       <c r="F26" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Con actualizaciones de junta 8
</commit_message>
<xml_diff>
--- a/swbproys/gestor-bsc/doc/LAU/formatos lanzamiento.xlsx
+++ b/swbproys/gestor-bsc/doc/LAU/formatos lanzamiento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="15240" windowHeight="5985" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="330" windowWidth="15240" windowHeight="5985" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="GOAL" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,18 @@
     <sheet name="INV" sheetId="9" r:id="rId9"/>
     <sheet name="Minuta Junta 6" sheetId="10" r:id="rId10"/>
     <sheet name="Minuta Junta 7" sheetId="11" r:id="rId11"/>
+    <sheet name="Minuta Junta 5" sheetId="12" r:id="rId12"/>
+    <sheet name="Minuta Junta 8" sheetId="13" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ITL Riesgos'!$A$4:$L$16</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="249">
   <si>
     <t>Measures</t>
   </si>
@@ -737,6 +742,60 @@
   </si>
   <si>
     <t>Diaria</t>
+  </si>
+  <si>
+    <t>Relanzamiento ciclo 2</t>
+  </si>
+  <si>
+    <t>CIRI, MEJS, JRJN</t>
+  </si>
+  <si>
+    <t>Meeting role</t>
+  </si>
+  <si>
+    <t>Quality goals</t>
+  </si>
+  <si>
+    <t>coach</t>
+  </si>
+  <si>
+    <t>estimate defects removed</t>
+  </si>
+  <si>
+    <t>estimate  defects inyected</t>
+  </si>
+  <si>
+    <t>produce the quality plan</t>
+  </si>
+  <si>
+    <t>launch meeting documentation</t>
+  </si>
+  <si>
+    <t>Generar la definición de defectos menores y defectos mayores</t>
+  </si>
+  <si>
+    <t>Junta 7. Producir un plan de calidad</t>
+  </si>
+  <si>
+    <t>Junta 8. Prepararse para la reunión con la gerencia</t>
+  </si>
+  <si>
+    <t>Carlos presentará las primeras 3 diapositivas de la presentación</t>
+  </si>
+  <si>
+    <t>Martha  presentará las primeras 3 diapositivas de la presentación</t>
+  </si>
+  <si>
+    <t>José  presentará las primeras 3 diapositivas de la presentación</t>
+  </si>
+  <si>
+    <t>Planning for the Management Meeting</t>
+  </si>
+  <si>
+    <t>lider</t>
+  </si>
+  <si>
+    <t>Management Meeting Preparation</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1329,6 +1388,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1347,6 +1434,15 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1359,28 +1455,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1685,7 +1759,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,14 +1790,14 @@
     <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="71"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="84" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1740,7 +1814,7 @@
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="85"/>
     </row>
     <row r="6" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
@@ -1817,7 +1891,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
         <v>150</v>
       </c>
@@ -1832,13 +1906,13 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1918,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,17 +2057,17 @@
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -2025,106 +2099,106 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="81"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="81"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="89"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
@@ -2239,7 +2313,9 @@
       <c r="B36" s="39">
         <v>0.8354166666666667</v>
       </c>
-      <c r="C36" s="39"/>
+      <c r="C36" s="39">
+        <v>0.84583333333333333</v>
+      </c>
       <c r="D36" s="54" t="s">
         <v>77</v>
       </c>
@@ -2273,55 +2349,86 @@
       <c r="B42" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="79" t="s">
+      <c r="C42" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="79"/>
+      <c r="D42" s="94"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
+      <c r="A43" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B43" s="79" t="s">
+        <v>232</v>
+      </c>
+      <c r="C43" s="91">
+        <v>41490</v>
+      </c>
+      <c r="D43" s="92"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="38"/>
       <c r="B44" s="38"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="77"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
@@ -2331,6 +2438,894 @@
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="37.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="40">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="40">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="69">
+        <v>0.5625</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="69">
+        <v>0.70486111111111116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="90" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="89"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="89"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="89"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="89"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="89"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="89"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="93"/>
+    </row>
+    <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="39">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="C29" s="39">
+        <v>0.5625</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="39">
+        <v>0.5625</v>
+      </c>
+      <c r="C30" s="39">
+        <v>0.56458333333333333</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="39">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="C31" s="39">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="39">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C32" s="39">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="49"/>
+      <c r="B33" s="39">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C33" s="39">
+        <v>0.70208333333333339</v>
+      </c>
+      <c r="D33" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="39">
+        <v>0.70277777777777783</v>
+      </c>
+      <c r="C34" s="39">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="49"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="49"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="94"/>
+    </row>
+    <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="38"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="38"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="37.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="40">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="40">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="69">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="69">
+        <v>0.91527777777777775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="90" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="89"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="89"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="89"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="89"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="89"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="89"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="93"/>
+    </row>
+    <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="39">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="C29" s="39">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="39">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="C30" s="39">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="39">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="C31" s="39">
+        <v>0.84861111111111109</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="39">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="C32" s="39">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="49"/>
+      <c r="B33" s="39">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="C33" s="39">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="D33" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="39">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="C34" s="39">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="39">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C35" s="39">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="D35" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="39">
+        <v>0.91388888888888886</v>
+      </c>
+      <c r="C36" s="39">
+        <v>0.91527777777777775</v>
+      </c>
+      <c r="D36" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="49"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="49"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="94"/>
+    </row>
+    <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="91">
+        <v>41432</v>
+      </c>
+      <c r="D42" s="92"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="38"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="A21:B21"/>
@@ -2349,24 +3344,24 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,7 +3392,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>44</v>
@@ -2419,54 +3414,54 @@
         <v>46</v>
       </c>
       <c r="B4" s="69">
-        <v>0.5625</v>
+        <v>0.9375</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="69">
-        <v>0.70486111111111116</v>
+        <v>5.4166666666666669E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="82" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="B7" s="90" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -2474,106 +3469,106 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="81"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="81"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="89"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
@@ -2595,92 +3590,84 @@
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49"/>
       <c r="B29" s="39">
-        <v>0.56180555555555556</v>
+        <v>0.9375</v>
       </c>
       <c r="C29" s="39">
-        <v>0.5625</v>
+        <v>0.93819444444444444</v>
       </c>
       <c r="D29" s="54" t="s">
-        <v>94</v>
+        <v>233</v>
       </c>
       <c r="E29" s="54" t="s">
-        <v>97</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="49"/>
       <c r="B30" s="39">
-        <v>0.5625</v>
+        <v>0.93819444444444444</v>
       </c>
       <c r="C30" s="39">
-        <v>0.56458333333333333</v>
+        <v>0.93958333333333333</v>
       </c>
       <c r="D30" s="54" t="s">
         <v>95</v>
       </c>
       <c r="E30" s="54" t="s">
-        <v>97</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49"/>
       <c r="B31" s="39">
-        <v>0.56527777777777777</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="C31" s="39">
-        <v>0.57638888888888895</v>
+        <v>0.99305555555555547</v>
       </c>
       <c r="D31" s="54" t="s">
-        <v>203</v>
+        <v>246</v>
       </c>
       <c r="E31" s="54" t="s">
-        <v>97</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="49"/>
       <c r="B32" s="39">
-        <v>0.64583333333333337</v>
+        <v>0.99375000000000002</v>
       </c>
       <c r="C32" s="39">
-        <v>0.69097222222222221</v>
+        <v>5.0694444444444452E-2</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
       <c r="E32" s="54" t="s">
-        <v>97</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49"/>
       <c r="B33" s="39">
-        <v>0.69097222222222221</v>
+        <v>5.0694444444444452E-2</v>
       </c>
       <c r="C33" s="39">
-        <v>0.70208333333333339</v>
+        <v>5.4166666666666669E-2</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>205</v>
+        <v>77</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>97</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="49"/>
-      <c r="B34" s="39">
-        <v>0.70277777777777783</v>
-      </c>
-      <c r="C34" s="39">
-        <v>0.70486111111111116</v>
-      </c>
-      <c r="D34" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="54" t="s">
-        <v>97</v>
-      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="49"/>
@@ -2711,60 +3698,64 @@
       <c r="E38" s="54"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="68" t="s">
+      <c r="A41" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="68" t="s">
+      <c r="B41" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="79" t="s">
+      <c r="C41" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="79"/>
-    </row>
-    <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
-        <v>204</v>
+      <c r="D41" s="94"/>
+    </row>
+    <row r="42" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="49" t="s">
+        <v>243</v>
       </c>
       <c r="B42" s="38"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+    </row>
+    <row r="43" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="49" t="s">
+        <v>244</v>
+      </c>
       <c r="B43" s="38"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+    </row>
+    <row r="44" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="49" t="s">
+        <v>245</v>
+      </c>
       <c r="B44" s="38"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="77"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -2804,7 +3795,6 @@
     <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3001,7 +3991,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>18</v>
       </c>
@@ -3013,7 +4003,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="52" t="s">
         <v>144</v>
@@ -3023,7 +4013,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>19</v>
       </c>
@@ -3035,7 +4025,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="53" t="s">
         <v>107</v>
@@ -3045,7 +4035,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>20</v>
       </c>
@@ -3235,10 +4225,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3257,29 +4248,29 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
     </row>
     <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
@@ -3294,10 +4285,10 @@
       <c r="D4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G4" s="25" t="s">
@@ -3323,10 +4314,10 @@
       <c r="A5" s="27">
         <v>1</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="73" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="74">
         <v>41424</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -3348,18 +4339,18 @@
       </c>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
-      <c r="L5" s="84" t="s">
+      <c r="L5" s="73" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>2</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="74">
         <v>41424</v>
       </c>
       <c r="D6" s="27" t="s">
@@ -3386,10 +4377,10 @@
       <c r="A7" s="27">
         <v>3</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="73" t="s">
         <v>214</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="74">
         <v>41424</v>
       </c>
       <c r="D7" s="27" t="s">
@@ -3411,7 +4402,7 @@
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="73" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3419,10 +4410,10 @@
       <c r="A8" s="27">
         <v>4</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="74">
         <v>41424</v>
       </c>
       <c r="D8" s="27" t="s">
@@ -3444,18 +4435,18 @@
       </c>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
-      <c r="L8" s="84" t="s">
+      <c r="L8" s="73" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>5</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="74">
         <v>41424</v>
       </c>
       <c r="D9" s="27" t="s">
@@ -3478,14 +4469,14 @@
       <c r="J9" s="27"/>
       <c r="K9" s="27"/>
     </row>
-    <row r="10" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>6</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="74">
         <v>41424</v>
       </c>
       <c r="D10" s="27" t="s">
@@ -3512,10 +4503,10 @@
       <c r="A11" s="27">
         <v>7</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="73" t="s">
         <v>220</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="74">
         <v>41424</v>
       </c>
       <c r="D11" s="27" t="s">
@@ -3537,7 +4528,7 @@
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
-      <c r="L11" s="84" t="s">
+      <c r="L11" s="73" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3545,10 +4536,10 @@
       <c r="A12" s="27">
         <v>8</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="85">
+      <c r="C12" s="74">
         <v>41424</v>
       </c>
       <c r="D12" s="27" t="s">
@@ -3570,7 +4561,7 @@
       </c>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
-      <c r="L12" s="84" t="s">
+      <c r="L12" s="73" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3578,10 +4569,10 @@
       <c r="A13" s="27">
         <v>9</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="C13" s="85">
+      <c r="C13" s="74">
         <v>41424</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -3603,18 +4594,18 @@
       </c>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="84" t="s">
+      <c r="L13" s="73" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>10</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="85">
+      <c r="C14" s="74">
         <v>41424</v>
       </c>
       <c r="D14" s="27" t="s">
@@ -3637,11 +4628,11 @@
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>11</v>
       </c>
-      <c r="B15" s="86"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -3655,7 +4646,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="28"/>
       <c r="C16" s="27"/>
@@ -3668,6 +4659,15 @@
       <c r="J16" s="27"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:L16">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="36"/>
+        <filter val="54"/>
+        <filter val="81"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="4">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="E2:H2"/>
@@ -3989,17 +4989,17 @@
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -4031,114 +5031,114 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="81"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="81"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="89"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81" t="s">
+      <c r="B17" s="88"/>
+      <c r="C17" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="81"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81" t="s">
+      <c r="B18" s="88"/>
+      <c r="C18" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="81"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
@@ -4296,10 +5296,10 @@
       <c r="B43" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="79"/>
+      <c r="D43" s="94"/>
     </row>
     <row r="44" spans="1:5" ht="153" x14ac:dyDescent="0.25">
       <c r="A44" s="38" t="s">
@@ -4308,10 +5308,10 @@
       <c r="B44" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="76">
+      <c r="C44" s="91">
         <v>41423</v>
       </c>
-      <c r="D44" s="77"/>
+      <c r="D44" s="92"/>
     </row>
     <row r="45" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A45" s="38" t="s">
@@ -4320,10 +5320,10 @@
       <c r="B45" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="77" t="s">
+      <c r="C45" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="77"/>
+      <c r="D45" s="92"/>
     </row>
     <row r="46" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A46" s="38" t="s">
@@ -4332,10 +5332,10 @@
       <c r="B46" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="76">
+      <c r="C46" s="91">
         <v>41423</v>
       </c>
-      <c r="D46" s="77"/>
+      <c r="D46" s="92"/>
     </row>
     <row r="47" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
@@ -4344,10 +5344,10 @@
       <c r="B47" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="76">
+      <c r="C47" s="91">
         <v>41421</v>
       </c>
-      <c r="D47" s="77"/>
+      <c r="D47" s="92"/>
     </row>
     <row r="48" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A48" s="38" t="s">
@@ -4356,13 +5356,38 @@
       <c r="B48" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="76">
+      <c r="C48" s="91">
         <v>41421</v>
       </c>
-      <c r="D48" s="77"/>
+      <c r="D48" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="B7:J7"/>
@@ -4370,31 +5395,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4471,17 +5471,17 @@
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -4513,106 +5513,106 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="81"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="81"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="89"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
@@ -4818,10 +5818,10 @@
       <c r="B43" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="79"/>
+      <c r="D43" s="94"/>
     </row>
     <row r="44" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A44" s="38" t="s">
@@ -4830,10 +5830,10 @@
       <c r="B44" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="77" t="s">
+      <c r="C44" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="D44" s="77"/>
+      <c r="D44" s="92"/>
     </row>
     <row r="45" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A45" s="38" t="s">
@@ -4842,68 +5842,43 @@
       <c r="B45" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="76">
+      <c r="C45" s="91">
         <v>41422</v>
       </c>
-      <c r="D45" s="77"/>
+      <c r="D45" s="92"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="92"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
+      <c r="C50" s="92"/>
+      <c r="D50" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
@@ -4913,6 +5888,31 @@
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4989,17 +5989,17 @@
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -5031,108 +6031,108 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="81"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="81"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="89"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="78"/>
-    </row>
-    <row r="28" spans="1:5" ht="28.15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="93"/>
+    </row>
+    <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
         <v>51</v>
       </c>
@@ -5149,7 +6149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="56">
         <v>0.3979166666666667</v>
@@ -5162,7 +6162,7 @@
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="56">
         <v>0.39999999999999997</v>
@@ -5175,7 +6175,7 @@
       </c>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="56">
         <v>0.4069444444444445</v>
@@ -5188,7 +6188,7 @@
       </c>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="56">
         <v>0.4826388888888889</v>
@@ -5201,7 +6201,7 @@
       </c>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="56">
         <v>0.64930555555555558</v>
@@ -5214,7 +6214,7 @@
       </c>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="56">
         <v>0.67986111111111114</v>
@@ -5227,7 +6227,7 @@
       </c>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="57">
         <v>0.38750000000000001</v>
@@ -5240,7 +6240,7 @@
       </c>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="57">
         <v>0.53749999999999998</v>
@@ -5253,7 +6253,7 @@
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="57">
         <v>0.65</v>
@@ -5266,7 +6266,7 @@
       </c>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="57">
         <v>0.74652777777777779</v>
@@ -5279,7 +6279,7 @@
       </c>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="57">
         <v>1.6666666666666666E-2</v>
@@ -5292,7 +6292,7 @@
       </c>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="59">
         <v>1.9444444444444445E-2</v>
@@ -5305,7 +6305,7 @@
       </c>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="49"/>
       <c r="B41" s="61">
         <v>2.5694444444444447E-2</v>
@@ -5345,10 +6345,10 @@
       <c r="B44" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="79" t="s">
+      <c r="C44" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="79"/>
+      <c r="D44" s="94"/>
     </row>
     <row r="45" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="38" t="s">
@@ -5357,10 +6357,10 @@
       <c r="B45" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="76">
+      <c r="C45" s="91">
         <v>41422</v>
       </c>
-      <c r="D45" s="77"/>
+      <c r="D45" s="92"/>
     </row>
     <row r="46" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A46" s="38" t="s">
@@ -5369,10 +6369,10 @@
       <c r="B46" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C46" s="76">
+      <c r="C46" s="91">
         <v>41422</v>
       </c>
-      <c r="D46" s="77"/>
+      <c r="D46" s="92"/>
     </row>
     <row r="47" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
@@ -5381,10 +6381,10 @@
       <c r="B47" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="76">
+      <c r="C47" s="91">
         <v>41422</v>
       </c>
-      <c r="D47" s="77"/>
+      <c r="D47" s="92"/>
     </row>
     <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A48" s="38" t="s">
@@ -5393,10 +6393,10 @@
       <c r="B48" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="76">
+      <c r="C48" s="91">
         <v>41422</v>
       </c>
-      <c r="D48" s="77"/>
+      <c r="D48" s="92"/>
     </row>
     <row r="49" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A49" s="38" t="s">
@@ -5405,10 +6405,10 @@
       <c r="B49" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="76">
+      <c r="C49" s="91">
         <v>41422</v>
       </c>
-      <c r="D49" s="77"/>
+      <c r="D49" s="92"/>
     </row>
     <row r="50" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A50" s="38" t="s">
@@ -5417,10 +6417,10 @@
       <c r="B50" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="76">
+      <c r="C50" s="91">
         <v>41422</v>
       </c>
-      <c r="D50" s="77"/>
+      <c r="D50" s="92"/>
     </row>
     <row r="51" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
@@ -5429,10 +6429,10 @@
       <c r="B51" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="76">
+      <c r="C51" s="91">
         <v>41422</v>
       </c>
-      <c r="D51" s="77"/>
+      <c r="D51" s="92"/>
     </row>
     <row r="52" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="38" t="s">
@@ -5441,10 +6441,10 @@
       <c r="B52" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="76">
+      <c r="C52" s="91">
         <v>41422</v>
       </c>
-      <c r="D52" s="77"/>
+      <c r="D52" s="92"/>
     </row>
     <row r="53" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A53" s="38" t="s">
@@ -5453,10 +6453,10 @@
       <c r="B53" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="76">
+      <c r="C53" s="91">
         <v>41422</v>
       </c>
-      <c r="D53" s="77"/>
+      <c r="D53" s="92"/>
     </row>
     <row r="54" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A54" s="38" t="s">
@@ -5465,10 +6465,10 @@
       <c r="B54" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="76">
+      <c r="C54" s="91">
         <v>41422</v>
       </c>
-      <c r="D54" s="77"/>
+      <c r="D54" s="92"/>
     </row>
     <row r="55" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A55" s="38" t="s">
@@ -5477,10 +6477,10 @@
       <c r="B55" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="76">
+      <c r="C55" s="91">
         <v>41422</v>
       </c>
-      <c r="D55" s="77"/>
+      <c r="D55" s="92"/>
     </row>
     <row r="56" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A56" s="38" t="s">
@@ -5489,10 +6489,10 @@
       <c r="B56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="76">
+      <c r="C56" s="91">
         <v>41422</v>
       </c>
-      <c r="D56" s="77"/>
+      <c r="D56" s="92"/>
     </row>
     <row r="57" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A57" s="38" t="s">
@@ -5501,10 +6501,10 @@
       <c r="B57" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C57" s="76">
+      <c r="C57" s="91">
         <v>41422</v>
       </c>
-      <c r="D57" s="77"/>
+      <c r="D57" s="92"/>
     </row>
     <row r="58" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A58" s="38" t="s">
@@ -5513,10 +6513,10 @@
       <c r="B58" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="76">
+      <c r="C58" s="91">
         <v>41422</v>
       </c>
-      <c r="D58" s="77"/>
+      <c r="D58" s="92"/>
     </row>
     <row r="59" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A59" s="38" t="s">
@@ -5525,10 +6525,10 @@
       <c r="B59" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="76">
+      <c r="C59" s="91">
         <v>41422</v>
       </c>
-      <c r="D59" s="77"/>
+      <c r="D59" s="92"/>
     </row>
     <row r="60" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A60" s="38" t="s">
@@ -5537,10 +6537,10 @@
       <c r="B60" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C60" s="76">
+      <c r="C60" s="91">
         <v>41422</v>
       </c>
-      <c r="D60" s="77"/>
+      <c r="D60" s="92"/>
     </row>
     <row r="61" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A61" s="38" t="s">
@@ -5549,10 +6549,10 @@
       <c r="B61" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="76">
+      <c r="C61" s="91">
         <v>41422</v>
       </c>
-      <c r="D61" s="77"/>
+      <c r="D61" s="92"/>
     </row>
     <row r="62" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" s="38" t="s">
@@ -5561,10 +6561,10 @@
       <c r="B62" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C62" s="76">
+      <c r="C62" s="91">
         <v>41422</v>
       </c>
-      <c r="D62" s="77"/>
+      <c r="D62" s="92"/>
     </row>
     <row r="63" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" s="38" t="s">
@@ -5573,10 +6573,10 @@
       <c r="B63" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C63" s="76">
+      <c r="C63" s="91">
         <v>41422</v>
       </c>
-      <c r="D63" s="77"/>
+      <c r="D63" s="92"/>
     </row>
     <row r="64" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A64" s="38" t="s">
@@ -5585,10 +6585,10 @@
       <c r="B64" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="76">
+      <c r="C64" s="91">
         <v>41422</v>
       </c>
-      <c r="D64" s="77"/>
+      <c r="D64" s="92"/>
     </row>
     <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A65" s="38" t="s">
@@ -5597,10 +6597,10 @@
       <c r="B65" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C65" s="76">
+      <c r="C65" s="91">
         <v>41422</v>
       </c>
-      <c r="D65" s="77"/>
+      <c r="D65" s="92"/>
     </row>
     <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A66" s="38" t="s">
@@ -5609,10 +6609,10 @@
       <c r="B66" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C66" s="76">
+      <c r="C66" s="91">
         <v>41422</v>
       </c>
-      <c r="D66" s="77"/>
+      <c r="D66" s="92"/>
     </row>
     <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A67" s="38" t="s">
@@ -5621,10 +6621,10 @@
       <c r="B67" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="76">
+      <c r="C67" s="91">
         <v>41422</v>
       </c>
-      <c r="D67" s="77"/>
+      <c r="D67" s="92"/>
     </row>
     <row r="68" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A68" s="38" t="s">
@@ -5633,10 +6633,10 @@
       <c r="B68" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C68" s="76">
+      <c r="C68" s="91">
         <v>41422</v>
       </c>
-      <c r="D68" s="77"/>
+      <c r="D68" s="92"/>
     </row>
     <row r="69" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A69" s="38" t="s">
@@ -5645,10 +6645,10 @@
       <c r="B69" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C69" s="76">
+      <c r="C69" s="91">
         <v>41422</v>
       </c>
-      <c r="D69" s="77"/>
+      <c r="D69" s="92"/>
     </row>
     <row r="70" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A70" s="38" t="s">
@@ -5657,10 +6657,10 @@
       <c r="B70" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C70" s="76">
+      <c r="C70" s="91">
         <v>41422</v>
       </c>
-      <c r="D70" s="77"/>
+      <c r="D70" s="92"/>
     </row>
     <row r="71" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="38" t="s">
@@ -5669,10 +6669,10 @@
       <c r="B71" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C71" s="76">
+      <c r="C71" s="91">
         <v>41422</v>
       </c>
-      <c r="D71" s="77"/>
+      <c r="D71" s="92"/>
     </row>
     <row r="72" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A72" s="38" t="s">
@@ -5681,10 +6681,10 @@
       <c r="B72" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C72" s="76">
+      <c r="C72" s="91">
         <v>41422</v>
       </c>
-      <c r="D72" s="77"/>
+      <c r="D72" s="92"/>
     </row>
     <row r="73" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A73" s="38" t="s">
@@ -5693,10 +6693,10 @@
       <c r="B73" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C73" s="76">
+      <c r="C73" s="91">
         <v>41422</v>
       </c>
-      <c r="D73" s="77"/>
+      <c r="D73" s="92"/>
     </row>
     <row r="74" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A74" s="38" t="s">
@@ -5705,10 +6705,10 @@
       <c r="B74" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="76">
+      <c r="C74" s="91">
         <v>41422</v>
       </c>
-      <c r="D74" s="77"/>
+      <c r="D74" s="92"/>
     </row>
     <row r="75" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A75" s="38" t="s">
@@ -5717,10 +6717,10 @@
       <c r="B75" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C75" s="76">
+      <c r="C75" s="91">
         <v>41422</v>
       </c>
-      <c r="D75" s="77"/>
+      <c r="D75" s="92"/>
     </row>
     <row r="76" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A76" s="38" t="s">
@@ -5729,10 +6729,10 @@
       <c r="B76" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="76">
+      <c r="C76" s="91">
         <v>41422</v>
       </c>
-      <c r="D76" s="77"/>
+      <c r="D76" s="92"/>
     </row>
     <row r="77" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A77" s="38" t="s">
@@ -5741,10 +6741,10 @@
       <c r="B77" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C77" s="76">
+      <c r="C77" s="91">
         <v>41422</v>
       </c>
-      <c r="D77" s="77"/>
+      <c r="D77" s="92"/>
     </row>
     <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A78" s="38" t="s">
@@ -5753,29 +6753,42 @@
       <c r="B78" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="C78" s="76" t="s">
+      <c r="C78" s="91" t="s">
         <v>164</v>
       </c>
-      <c r="D78" s="77"/>
+      <c r="D78" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="C61:D61"/>
@@ -5792,35 +6805,22 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5898,17 +6898,17 @@
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="90" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -5940,106 +6940,106 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="81"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="81"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="89"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
@@ -6199,10 +7199,10 @@
       <c r="B43" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="79"/>
+      <c r="D43" s="94"/>
     </row>
     <row r="44" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="38" t="s">
@@ -6211,65 +7211,47 @@
       <c r="B44" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="77"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="92"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
+      <c r="C50" s="92"/>
+      <c r="D50" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
@@ -6286,6 +7268,24 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6293,7 +7293,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
@@ -6313,26 +7313,26 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:7" s="76" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="77" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6533,7 +7533,7 @@
       <c r="C14" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="78">
         <v>41453</v>
       </c>
       <c r="F14" t="s">
@@ -6543,7 +7543,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -6553,14 +7553,14 @@
       <c r="C15" t="s">
         <v>229</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D15" s="78">
         <v>41432</v>
       </c>
       <c r="F15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -6570,7 +7570,7 @@
       <c r="C16" t="s">
         <v>229</v>
       </c>
-      <c r="D16" s="89">
+      <c r="D16" s="78">
         <v>41439</v>
       </c>
       <c r="F16" t="s">
@@ -6587,15 +7587,14 @@
       <c r="C17" t="s">
         <v>229</v>
       </c>
-      <c r="D17" s="89">
+      <c r="D17" s="78">
         <v>41432</v>
       </c>
       <c r="F17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -6605,7 +7604,7 @@
       <c r="C21" t="s">
         <v>229</v>
       </c>
-      <c r="D21" s="89">
+      <c r="D21" s="78">
         <v>41432</v>
       </c>
       <c r="F21" t="s">
@@ -6622,7 +7621,7 @@
       <c r="C22" t="s">
         <v>229</v>
       </c>
-      <c r="D22" s="89">
+      <c r="D22" s="78">
         <v>41439</v>
       </c>
       <c r="F22" t="s">
@@ -6651,7 +7650,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>162</v>
       </c>
@@ -6673,14 +7672,6 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:6" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>